<commit_message>
completed plots filtered age
</commit_message>
<xml_diff>
--- a/results/by_outcome/full_results_education_PGI.xlsx
+++ b/results/by_outcome/full_results_education_PGI.xlsx
@@ -471,32 +471,32 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>0.636578570169278</v>
+        <v>0.675903707073575</v>
       </c>
       <c r="D2" t="n">
-        <v>0.363621994933512</v>
+        <v>0.324438889402782</v>
       </c>
       <c r="E2" t="n">
-        <v>1.00020056510279</v>
+        <v>1.00034259647636</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2" t="n">
-        <v>0.363549079674978</v>
+        <v>0.324327775849591</v>
       </c>
       <c r="K2" t="n">
-        <v>0.319632137160595</v>
+        <v>0.287203319078383</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0174156220483999</v>
+        <v>0.00933406479094052</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0462239888175782</v>
+        <v>0.034262491581737</v>
       </c>
       <c r="N2" t="n">
-        <v>0.337047759208995</v>
+        <v>0.296537383869324</v>
       </c>
       <c r="O2"/>
     </row>
@@ -511,10 +511,10 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" t="n">
-        <v>0.607764425447057</v>
+        <v>0.650966739891599</v>
       </c>
       <c r="G3" t="n">
-        <v>0.319696244213039</v>
+        <v>0.287301713923497</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -538,10 +538,10 @@
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4" t="n">
-        <v>0.590345310432631</v>
+        <v>0.641629477282951</v>
       </c>
       <c r="I4" t="n">
-        <v>0.295417105330435</v>
+        <v>0.241756267272275</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
@@ -549,7 +549,7 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="n">
-        <v>0.409773068492556</v>
+        <v>0.358590267431328</v>
       </c>
     </row>
   </sheetData>
@@ -594,16 +594,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.363549079674978</v>
+        <v>0.324327775849591</v>
       </c>
       <c r="D2" t="n">
-        <v>0.323649872339535</v>
+        <v>0.264162236920513</v>
       </c>
       <c r="E2" t="n">
-        <v>0.40344828701042</v>
+        <v>0.38449331477867</v>
       </c>
       <c r="F2" t="n">
-        <v>1814</v>
+        <v>948</v>
       </c>
     </row>
     <row r="3">
@@ -614,16 +614,16 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.337047759208995</v>
+        <v>0.296537383869324</v>
       </c>
       <c r="D3" t="n">
-        <v>0.294393424007225</v>
+        <v>0.217012782397054</v>
       </c>
       <c r="E3" t="n">
-        <v>0.379702094410765</v>
+        <v>0.376061985341593</v>
       </c>
       <c r="F3" t="n">
-        <v>1814</v>
+        <v>948</v>
       </c>
     </row>
     <row r="4">
@@ -634,16 +634,16 @@
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>0.409773068492556</v>
+        <v>0.358590267431328</v>
       </c>
       <c r="D4" t="n">
-        <v>0.371958559678431</v>
+        <v>0.279364345887865</v>
       </c>
       <c r="E4" t="n">
-        <v>0.447587577306681</v>
+        <v>0.437816188974792</v>
       </c>
       <c r="F4" t="n">
-        <v>1814</v>
+        <v>948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>